<commit_message>
refactor: regenerate some figures
</commit_message>
<xml_diff>
--- a/8_annotation_error_study/results/etude-erreur-simulation-evolution-accord-entre-clusterings.xlsx
+++ b/8_annotation_error_study/results/etude-erreur-simulation-evolution-accord-entre-clusterings.xlsx
@@ -46,22 +46,22 @@
     <t>constraints_needed</t>
   </si>
   <si>
-    <t>error:0.00%</t>
-  </si>
-  <si>
-    <t>error:5.00%</t>
-  </si>
-  <si>
-    <t>error:10.00%</t>
-  </si>
-  <si>
-    <t>error:15.00%</t>
-  </si>
-  <si>
-    <t>error:20.00%</t>
-  </si>
-  <si>
-    <t>error:25.00%</t>
+    <t>diff:0.00%</t>
+  </si>
+  <si>
+    <t>diff:5.00%</t>
+  </si>
+  <si>
+    <t>diff:10.00%</t>
+  </si>
+  <si>
+    <t>diff:15.00%</t>
+  </si>
+  <si>
+    <t>diff:20.00%</t>
+  </si>
+  <si>
+    <t>diff:25.00%</t>
   </si>
   <si>
     <t>97.46 (+/-0.65)</t>

</xml_diff>

<commit_message>
refactor: fix similitude computations annotation error study
</commit_message>
<xml_diff>
--- a/8_annotation_error_study/results/etude-erreur-simulation-evolution-accord-entre-clusterings.xlsx
+++ b/8_annotation_error_study/results/etude-erreur-simulation-evolution-accord-entre-clusterings.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="62">
   <si>
     <t>size:1000</t>
   </si>
@@ -64,166 +64,142 @@
     <t>diff:25.00%</t>
   </si>
   <si>
-    <t>97.46 (+/-0.65)</t>
-  </si>
-  <si>
-    <t>85.10 (+/-1.85)</t>
-  </si>
-  <si>
-    <t>79.29 (+/-3.06)</t>
-  </si>
-  <si>
-    <t>73.67 (+/-4.08)</t>
-  </si>
-  <si>
-    <t>68.86 (+/-4.59)</t>
-  </si>
-  <si>
-    <t>64.89 (+/-5.15)</t>
-  </si>
-  <si>
-    <t>96.17 (+/-0.99)</t>
-  </si>
-  <si>
-    <t>76.76 (+/-0.95)</t>
-  </si>
-  <si>
-    <t>65.03 (+/-1.06)</t>
-  </si>
-  <si>
-    <t>57.84 (+/-1.14)</t>
-  </si>
-  <si>
-    <t>51.28 (+/-1.15)</t>
-  </si>
-  <si>
-    <t>43.63 (+/-1.12)</t>
-  </si>
-  <si>
-    <t>95.03 (+/-1.08)</t>
-  </si>
-  <si>
-    <t>77.85 (+/-0.78)</t>
-  </si>
-  <si>
-    <t>65.46 (+/-0.78)</t>
-  </si>
-  <si>
-    <t>56.21 (+/-0.97)</t>
-  </si>
-  <si>
-    <t>48.21 (+/-1.10)</t>
-  </si>
-  <si>
-    <t>39.60 (+/-0.97)</t>
-  </si>
-  <si>
-    <t>95.58 (+/-0.79)</t>
-  </si>
-  <si>
-    <t>73.50 (+/-0.81)</t>
-  </si>
-  <si>
-    <t>60.45 (+/-0.76)</t>
-  </si>
-  <si>
-    <t>50.50 (+/-0.72)</t>
-  </si>
-  <si>
-    <t>41.58 (+/-0.47)</t>
-  </si>
-  <si>
-    <t>35.70 (+/-0.47)</t>
-  </si>
-  <si>
-    <t>95.42 (+/-0.84)</t>
-  </si>
-  <si>
-    <t>73.34 (+/-0.57)</t>
-  </si>
-  <si>
-    <t>60.59 (+/-0.51)</t>
-  </si>
-  <si>
-    <t>47.56 (+/-0.98)</t>
-  </si>
-  <si>
-    <t>40.99 (+/-0.94)</t>
-  </si>
-  <si>
-    <t>34.94 (+/-0.57)</t>
-  </si>
-  <si>
-    <t>94.75 (+/-1.43)</t>
-  </si>
-  <si>
-    <t>73.50 (+/-1.01)</t>
-  </si>
-  <si>
-    <t>60.32 (+/-0.99)</t>
-  </si>
-  <si>
-    <t>51.65 (+/-1.04)</t>
-  </si>
-  <si>
-    <t>43.00 (+/-0.84)</t>
-  </si>
-  <si>
-    <t>37.00 (+/-0.99)</t>
-  </si>
-  <si>
-    <t>94.74 (+/-1.12)</t>
-  </si>
-  <si>
-    <t>70.74 (+/-0.47)</t>
-  </si>
-  <si>
-    <t>57.15 (+/-0.68)</t>
-  </si>
-  <si>
-    <t>48.16 (+/-0.74)</t>
-  </si>
-  <si>
-    <t>40.18 (+/-0.90)</t>
-  </si>
-  <si>
-    <t>32.12 (+/-0.70)</t>
-  </si>
-  <si>
-    <t>96.00 (+/-0.78)</t>
-  </si>
-  <si>
-    <t>68.97 (+/-0.58)</t>
-  </si>
-  <si>
-    <t>53.34 (+/-0.84)</t>
-  </si>
-  <si>
-    <t>41.68 (+/-0.65)</t>
-  </si>
-  <si>
-    <t>34.41 (+/-0.54)</t>
-  </si>
-  <si>
-    <t>26.49 (+/-0.72)</t>
-  </si>
-  <si>
-    <t>93.15 (+/-1.23)</t>
-  </si>
-  <si>
-    <t>68.72 (+/-1.31)</t>
-  </si>
-  <si>
-    <t>55.55 (+/-1.50)</t>
-  </si>
-  <si>
-    <t>46.29 (+/-1.37)</t>
-  </si>
-  <si>
-    <t>38.37 (+/-1.05)</t>
-  </si>
-  <si>
-    <t>31.24 (+/-1.11)</t>
+    <t>100.00 (+/-0.00)</t>
+  </si>
+  <si>
+    <t>86.16 (+/-3.52)</t>
+  </si>
+  <si>
+    <t>79.84 (+/-6.22)</t>
+  </si>
+  <si>
+    <t>73.94 (+/-8.48)</t>
+  </si>
+  <si>
+    <t>68.96 (+/-9.61)</t>
+  </si>
+  <si>
+    <t>65.05 (+/-10.78)</t>
+  </si>
+  <si>
+    <t>78.56 (+/-1.50)</t>
+  </si>
+  <si>
+    <t>66.02 (+/-2.00)</t>
+  </si>
+  <si>
+    <t>58.64 (+/-2.21)</t>
+  </si>
+  <si>
+    <t>51.92 (+/-2.30)</t>
+  </si>
+  <si>
+    <t>44.12 (+/-2.30)</t>
+  </si>
+  <si>
+    <t>80.09 (+/-1.27)</t>
+  </si>
+  <si>
+    <t>66.95 (+/-1.46)</t>
+  </si>
+  <si>
+    <t>57.13 (+/-1.97)</t>
+  </si>
+  <si>
+    <t>48.85 (+/-2.31)</t>
+  </si>
+  <si>
+    <t>40.19 (+/-2.01)</t>
+  </si>
+  <si>
+    <t>74.81 (+/-1.62)</t>
+  </si>
+  <si>
+    <t>61.13 (+/-1.55)</t>
+  </si>
+  <si>
+    <t>51.01 (+/-1.43)</t>
+  </si>
+  <si>
+    <t>42.01 (+/-0.96)</t>
+  </si>
+  <si>
+    <t>35.88 (+/-0.98)</t>
+  </si>
+  <si>
+    <t>75.06 (+/-1.02)</t>
+  </si>
+  <si>
+    <t>61.64 (+/-1.05)</t>
+  </si>
+  <si>
+    <t>48.25 (+/-2.14)</t>
+  </si>
+  <si>
+    <t>41.57 (+/-2.00)</t>
+  </si>
+  <si>
+    <t>35.31 (+/-1.25)</t>
+  </si>
+  <si>
+    <t>74.72 (+/-1.84)</t>
+  </si>
+  <si>
+    <t>60.93 (+/-1.92)</t>
+  </si>
+  <si>
+    <t>52.33 (+/-2.04)</t>
+  </si>
+  <si>
+    <t>43.37 (+/-1.71)</t>
+  </si>
+  <si>
+    <t>37.31 (+/-2.04)</t>
+  </si>
+  <si>
+    <t>71.86 (+/-0.91)</t>
+  </si>
+  <si>
+    <t>57.70 (+/-1.52)</t>
+  </si>
+  <si>
+    <t>48.52 (+/-1.61)</t>
+  </si>
+  <si>
+    <t>40.56 (+/-1.94)</t>
+  </si>
+  <si>
+    <t>32.47 (+/-1.46)</t>
+  </si>
+  <si>
+    <t>70.07 (+/-1.29)</t>
+  </si>
+  <si>
+    <t>54.00 (+/-1.84)</t>
+  </si>
+  <si>
+    <t>42.13 (+/-1.43)</t>
+  </si>
+  <si>
+    <t>34.87 (+/-1.15)</t>
+  </si>
+  <si>
+    <t>26.73 (+/-1.56)</t>
+  </si>
+  <si>
+    <t>71.03 (+/-3.09)</t>
+  </si>
+  <si>
+    <t>57.01 (+/-3.65)</t>
+  </si>
+  <si>
+    <t>47.41 (+/-3.27)</t>
+  </si>
+  <si>
+    <t>39.08 (+/-2.51)</t>
+  </si>
+  <si>
+    <t>31.90 (+/-2.56)</t>
   </si>
 </sst>
 </file>
@@ -656,28 +632,28 @@
         <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="E3" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="G3" t="s">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="H3" t="s">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="I3" t="s">
-        <v>58</v>
+        <v>16</v>
       </c>
       <c r="J3" t="s">
-        <v>64</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -688,28 +664,28 @@
         <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G4" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" t="s">
         <v>47</v>
       </c>
-      <c r="H4" t="s">
-        <v>53</v>
-      </c>
       <c r="I4" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="J4" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -720,28 +696,28 @@
         <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G5" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" t="s">
         <v>48</v>
       </c>
-      <c r="H5" t="s">
-        <v>54</v>
-      </c>
       <c r="I5" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="J5" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -752,28 +728,28 @@
         <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H6" t="s">
         <v>49</v>
       </c>
-      <c r="H6" t="s">
-        <v>55</v>
-      </c>
       <c r="I6" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="J6" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -784,28 +760,28 @@
         <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E7" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7" t="s">
         <v>50</v>
       </c>
-      <c r="H7" t="s">
-        <v>56</v>
-      </c>
       <c r="I7" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="J7" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -816,28 +792,28 @@
         <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="F8" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="G8" t="s">
+        <v>46</v>
+      </c>
+      <c r="H8" t="s">
         <v>51</v>
       </c>
-      <c r="H8" t="s">
-        <v>57</v>
-      </c>
       <c r="I8" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="J8" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>